<commit_message>
Update to 2021 min road ef and misc (#429)
* Update min EF pathways for road transport
* Update on-road diesel S standards
* Loop twice to output derived BC/OC from transportation and full EPA BC data (including country total) as well.
* Add new BC/OC residential-commertial EFs to match NEI. Add commercial cooking BC/OC from NEI, extended back to 1960
* Update US values to match 2023 EQUATES results
* Add writeout of BC total and by sector emissions from inventory
* Modifying India transport sector EF extension from 2020 to lower diesel NOx EF decline

---------

Co-authored-by: Hamza Ahsan <hamza.ahsan@pnnl.gov>
Co-authored-by: Noah Prime <noahprime21@gmail.com>
</commit_message>
<xml_diff>
--- a/input/emissions-inventories/PM25_Inventory.xlsx
+++ b/input/emissions-inventories/PM25_Inventory.xlsx
@@ -1,26 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11210"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orou913\Desktop\CEDS-Repositories\CEDS_version_comp\CEDS\input\emissions-inventories\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d3k117/Documents/Information &amp; Documents/CEDS_Project/CEDS/input/emissions-inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC82B75-A8F9-42B3-933F-3C07D5BC3D27}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B2E38D-FEF2-7846-8BBE-23A57D24224B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="345" windowWidth="24105" windowHeight="14535" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="940" yWindow="760" windowWidth="24100" windowHeight="14540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PM25_compare" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -876,19 +881,19 @@
   <dimension ref="A1:AO41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="AD2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="AB2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AQ10" sqref="AQ10"/>
+      <selection pane="bottomRight" activeCell="N4" sqref="N4:AL4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="39" max="39" width="16.375" customWidth="1"/>
-    <col min="40" max="40" width="15.875" customWidth="1"/>
+    <col min="39" max="39" width="16.33203125" customWidth="1"/>
+    <col min="40" max="40" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1013,7 +1018,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -1139,7 +1144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -1265,7 +1270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>117</v>
       </c>
@@ -1306,83 +1311,83 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>106.14239999999999</v>
+        <v>177.66406130332712</v>
       </c>
       <c r="O4">
-        <v>107.9568</v>
+        <v>180.70105380423871</v>
       </c>
       <c r="P4">
-        <v>108.4104</v>
+        <v>181.4603019294666</v>
       </c>
       <c r="Q4">
-        <v>130.63679999999999</v>
+        <v>218.66346006563339</v>
       </c>
       <c r="R4">
-        <v>122.9256</v>
+        <v>205.75624193675921</v>
       </c>
       <c r="S4">
-        <v>112.03919999999999</v>
+        <v>187.53428693128973</v>
       </c>
       <c r="T4">
-        <v>193.57788239999999</v>
+        <v>324.0159706741307</v>
       </c>
       <c r="U4">
-        <v>199.18074960000001</v>
+        <v>333.39420351694565</v>
       </c>
       <c r="V4">
-        <v>208.3357584</v>
+        <v>348.71810842842024</v>
       </c>
       <c r="W4">
-        <v>199.4923728</v>
+        <v>333.91580697897717</v>
       </c>
       <c r="X4">
-        <v>151.26471359999999</v>
+        <v>253.19102780849707</v>
       </c>
       <c r="Y4">
-        <v>151.4506896</v>
+        <v>253.50231953984053</v>
       </c>
       <c r="Z4">
-        <v>121.655410056487</v>
+        <v>204.06679832</v>
       </c>
       <c r="AA4">
-        <v>121.386812588531</v>
+        <v>202.26893871999999</v>
       </c>
       <c r="AB4">
-        <v>121.00250879797299</v>
+        <v>202.35532724000001</v>
       </c>
       <c r="AC4">
-        <v>120.503212627324</v>
+        <v>202.35532724000001</v>
       </c>
       <c r="AD4">
-        <v>111.430295660369</v>
+        <v>202.35657230999999</v>
       </c>
       <c r="AE4">
-        <v>102.357378693415</v>
+        <v>202.28164340000001</v>
       </c>
       <c r="AF4">
-        <v>93.220864050924504</v>
+        <v>202.28164340000001</v>
       </c>
       <c r="AG4">
-        <v>87.079587734450001</v>
+        <v>202.28191641000001</v>
       </c>
       <c r="AH4">
-        <v>80.938311417975001</v>
+        <v>202.27903229</v>
       </c>
       <c r="AI4">
-        <v>74.797035101500001</v>
+        <v>202.76924987000001</v>
       </c>
       <c r="AJ4">
-        <v>74.797035101500001</v>
+        <v>202.82113631999999</v>
       </c>
       <c r="AK4">
-        <v>74.797035101500001</v>
+        <v>202.88598726000001</v>
       </c>
       <c r="AL4">
-        <v>74.797035101500001</v>
+        <v>202.85367769000001</v>
       </c>
       <c r="AM4">
         <f t="shared" si="0"/>
-        <v>80.938311417975001</v>
+        <v>202.27903229</v>
       </c>
       <c r="AN4" s="4">
         <v>1</v>
@@ -1391,7 +1396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>83</v>
       </c>
@@ -1514,7 +1519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -1640,7 +1645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>69</v>
       </c>
@@ -1766,7 +1771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>67</v>
       </c>
@@ -1892,7 +1897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>81</v>
       </c>
@@ -2018,7 +2023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>113</v>
       </c>
@@ -2144,7 +2149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>75</v>
       </c>
@@ -2270,7 +2275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>101</v>
       </c>
@@ -2396,7 +2401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>99</v>
       </c>
@@ -2522,7 +2527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>55</v>
       </c>
@@ -2648,7 +2653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>65</v>
       </c>
@@ -2774,7 +2779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>107</v>
       </c>
@@ -2898,7 +2903,7 @@
       </c>
       <c r="AO16" s="4"/>
     </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>59</v>
       </c>
@@ -3024,7 +3029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>93</v>
       </c>
@@ -3145,7 +3150,7 @@
       </c>
       <c r="AO18" s="4"/>
     </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>105</v>
       </c>
@@ -3269,7 +3274,7 @@
       </c>
       <c r="AO19" s="4"/>
     </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>61</v>
       </c>
@@ -3395,7 +3400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>91</v>
       </c>
@@ -3519,7 +3524,7 @@
       </c>
       <c r="AO21" s="4"/>
     </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>63</v>
       </c>
@@ -3640,7 +3645,7 @@
       </c>
       <c r="AO22" s="4"/>
     </row>
-    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>97</v>
       </c>
@@ -3766,7 +3771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -3892,7 +3897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>111</v>
       </c>
@@ -4016,7 +4021,7 @@
       </c>
       <c r="AO25" s="4"/>
     </row>
-    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -4140,7 +4145,7 @@
       </c>
       <c r="AO26" s="4"/>
     </row>
-    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>77</v>
       </c>
@@ -4264,7 +4269,7 @@
       </c>
       <c r="AO27" s="4"/>
     </row>
-    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>115</v>
       </c>
@@ -4388,7 +4393,7 @@
       </c>
       <c r="AO28" s="4"/>
     </row>
-    <row r="29" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>47</v>
       </c>
@@ -4512,7 +4517,7 @@
       </c>
       <c r="AO29" s="4"/>
     </row>
-    <row r="30" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>103</v>
       </c>
@@ -4638,7 +4643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>73</v>
       </c>
@@ -4759,7 +4764,7 @@
       </c>
       <c r="AO31" s="4"/>
     </row>
-    <row r="32" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>89</v>
       </c>
@@ -4883,7 +4888,7 @@
       </c>
       <c r="AO32" s="4"/>
     </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -5003,7 +5008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -5123,7 +5128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>49</v>
       </c>
@@ -5243,7 +5248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>71</v>
       </c>
@@ -5363,7 +5368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>79</v>
       </c>
@@ -5483,7 +5488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>85</v>
       </c>
@@ -5603,7 +5608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>87</v>
       </c>
@@ -5723,7 +5728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>95</v>
       </c>
@@ -5843,7 +5848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>109</v>
       </c>

</xml_diff>